<commit_message>
update due to fix on validation error
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-no-basis-AppointmentResponse.xlsx
+++ b/output/StructureDefinition-no-basis-AppointmentResponse.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-24T14:49:19+02:00</t>
+    <t>2023-08-24T15:39:37+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -140,7 +140,7 @@
   </si>
   <si>
     <t>apr-1:Either the participantType or actor must be specified {participantType.exists() or actor.exists()}
-dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-1:The 'shortNotice' extension can only be used when the 'actor' is of type 'Patient'. {extension.where(url = 'no-basis-shortnotice').value.exists() and actor.type.value = 'Patient'}</t>
+dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-1:The 'shortNotice' extension can only be used when the 'actor' is of type 'Patient'. {extension.where(url = 'http://hl7.no/fhir/StructureDefinition/no-basis-shortnotice').value.exists() and actor.type.value = 'Patient'}</t>
   </si>
   <si>
     <t>Request</t>

</xml_diff>